<commit_message>
add solution 2 using two pointers version 1
</commit_message>
<xml_diff>
--- a/LC-simulation.xlsx
+++ b/LC-simulation.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjrCe\Desktop\CARL\repos\daily\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC56285D-2F2D-4EF1-AE77-54D418DF2589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5387A5E2-79ED-4DB5-9CE8-05DA4F266A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A7D1033-BAE6-4CC0-8EC1-C3CEB428B472}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{9A7D1033-BAE6-4CC0-8EC1-C3CEB428B472}"/>
   </bookViews>
   <sheets>
     <sheet name="88" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="21">
   <si>
     <t>[1,2,3,0,0,0]</t>
   </si>
@@ -93,6 +94,12 @@
   </si>
   <si>
     <t>88. Merge Sorted Array</t>
+  </si>
+  <si>
+    <t>i=0</t>
+  </si>
+  <si>
+    <t>j=0</t>
   </si>
 </sst>
 </file>
@@ -121,7 +128,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +183,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -204,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -243,9 +262,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,7 +580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFC02A0-2AA8-40C6-8E28-F3C19BE4F9B1}">
   <dimension ref="B1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -839,7 +857,7 @@
       <c r="D12" s="3">
         <v>1</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="3">
         <v>2</v>
       </c>
       <c r="F12" s="11">
@@ -851,7 +869,7 @@
       <c r="H12" s="13">
         <v>0</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="3">
         <v>6</v>
       </c>
       <c r="J12" s="3" t="s">
@@ -874,7 +892,7 @@
       <c r="E13" s="9">
         <v>5</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="3">
         <v>6</v>
       </c>
       <c r="G13" s="3"/>
@@ -928,7 +946,7 @@
       <c r="D16" s="3">
         <v>1</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="3">
         <v>2</v>
       </c>
       <c r="F16" s="11">
@@ -937,10 +955,10 @@
       <c r="G16" s="13">
         <v>0</v>
       </c>
-      <c r="H16" s="14">
-        <v>5</v>
-      </c>
-      <c r="I16" s="14">
+      <c r="H16" s="3">
+        <v>5</v>
+      </c>
+      <c r="I16" s="3">
         <v>6</v>
       </c>
       <c r="J16" s="3" t="s">
@@ -960,10 +978,10 @@
       <c r="D17" s="9">
         <v>2</v>
       </c>
-      <c r="E17" s="14">
-        <v>5</v>
-      </c>
-      <c r="F17" s="14">
+      <c r="E17" s="3">
+        <v>5</v>
+      </c>
+      <c r="F17" s="3">
         <v>6</v>
       </c>
       <c r="G17" s="3"/>
@@ -1026,10 +1044,10 @@
       <c r="G20" s="3">
         <v>3</v>
       </c>
-      <c r="H20" s="14">
-        <v>5</v>
-      </c>
-      <c r="I20" s="14">
+      <c r="H20" s="3">
+        <v>5</v>
+      </c>
+      <c r="I20" s="3">
         <v>6</v>
       </c>
       <c r="J20" s="3" t="s">
@@ -1049,10 +1067,10 @@
       <c r="D21" s="9">
         <v>2</v>
       </c>
-      <c r="E21" s="14">
-        <v>5</v>
-      </c>
-      <c r="F21" s="14">
+      <c r="E21" s="3">
+        <v>5</v>
+      </c>
+      <c r="F21" s="3">
         <v>6</v>
       </c>
       <c r="G21" s="3"/>
@@ -1109,16 +1127,16 @@
       <c r="E24" s="13">
         <v>2</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="3">
         <v>2</v>
       </c>
       <c r="G24" s="3">
         <v>3</v>
       </c>
-      <c r="H24" s="14">
-        <v>5</v>
-      </c>
-      <c r="I24" s="14">
+      <c r="H24" s="3">
+        <v>5</v>
+      </c>
+      <c r="I24" s="3">
         <v>6</v>
       </c>
       <c r="J24" s="3"/>
@@ -1133,13 +1151,13 @@
       <c r="C25" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="14">
-        <v>2</v>
-      </c>
-      <c r="E25" s="14">
-        <v>5</v>
-      </c>
-      <c r="F25" s="14">
+      <c r="D25" s="3">
+        <v>2</v>
+      </c>
+      <c r="E25" s="3">
+        <v>5</v>
+      </c>
+      <c r="F25" s="3">
         <v>6</v>
       </c>
       <c r="G25" s="3"/>
@@ -1157,4 +1175,181 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D138444-9AEE-49E4-A3F5-8181A2F9C510}">
+  <dimension ref="C4:K26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E10" s="15"/>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="F14" s="15"/>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>12</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="F18" s="15"/>
+    </row>
+    <row r="20" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="I20" s="14"/>
+    </row>
+    <row r="21" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+      <c r="I21">
+        <v>12</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="G22" s="15"/>
+    </row>
+    <row r="24" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <v>12</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+      <c r="I25">
+        <v>12</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="H26" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>